<commit_message>
bugfixes, it works now!!
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CBE90E-03B8-4496-BC11-C07EFCDCF9B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0233A50-9AFD-40F7-9DC3-7A88B701D3A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>analysis</t>
   </si>
@@ -263,10 +263,10 @@
     <t>When choosing for network based on shapefile indicate shapefile for analysis.  Provide name of shapefile. No extension needed.</t>
   </si>
   <si>
-    <t>NL332.osm</t>
-  </si>
-  <si>
     <t>name_of_pbf</t>
+  </si>
+  <si>
+    <t>zuidholland_4326</t>
   </si>
 </sst>
 </file>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +762,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -830,19 +830,23 @@
         <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
-        <v>75</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -1117,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8FA5B4-8351-441E-BC93-E5502E84268F}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1165,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Incorporated cutting in create_network_from_osm_dump.py Added a check for existing G_simple and edges_complex.p -> needs check. Added criticality_single_link_osm_rws to analyses_indirect.py -> now criticality_single_link_osm_rws is default, should be changed to criticality_single_link_osm when using for different project.
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ce\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RA2CE_Sprint\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0233A50-9AFD-40F7-9DC3-7A88B701D3A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C59A46-5992-49FD-A078-1196EACA34BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -251,9 +251,6 @@
     <t xml:space="preserve">name of the unique ID column if the hazard data is a shapefile and the data can be joined with the network by ID </t>
   </si>
   <si>
-    <t>test2</t>
-  </si>
-  <si>
     <t>When choosing network_source based on OSM dump. Provide name of *.pbf dump. No extension needed.</t>
   </si>
   <si>
@@ -266,7 +263,10 @@
     <t>name_of_pbf</t>
   </si>
   <si>
-    <t>zuidholland_4326</t>
+    <t>NL_with_margin_from_EU_dump.osm.pbf</t>
+  </si>
+  <si>
+    <t>TestNL</t>
   </si>
 </sst>
 </file>
@@ -715,37 +715,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.54296875" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
-    <col min="15" max="16" width="22.21875" customWidth="1"/>
-    <col min="17" max="17" width="21.77734375" customWidth="1"/>
-    <col min="18" max="18" width="20.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" customWidth="1"/>
+    <col min="15" max="16" width="22.1796875" customWidth="1"/>
+    <col min="17" max="17" width="21.81640625" customWidth="1"/>
+    <col min="18" max="18" width="20.6328125" customWidth="1"/>
+    <col min="19" max="19" width="16.90625" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="17.88671875" customWidth="1"/>
-    <col min="22" max="22" width="26.33203125" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" customWidth="1"/>
+    <col min="21" max="21" width="17.90625" customWidth="1"/>
+    <col min="22" max="22" width="26.36328125" customWidth="1"/>
+    <col min="23" max="23" width="13.6328125" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -762,7 +762,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -819,9 +819,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -830,12 +830,12 @@
         <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -859,7 +859,7 @@
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -885,7 +885,7 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -973,16 +973,16 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1125,34 +1125,34 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.08984375" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
+    <col min="8" max="8" width="22.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.21875" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="14" max="14" width="22.6328125" customWidth="1"/>
     <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="16.77734375" customWidth="1"/>
-    <col min="18" max="18" width="19.44140625" customWidth="1"/>
-    <col min="19" max="19" width="17.109375" customWidth="1"/>
-    <col min="20" max="20" width="19.44140625" customWidth="1"/>
-    <col min="21" max="21" width="19.33203125" customWidth="1"/>
-    <col min="22" max="22" width="17.21875" customWidth="1"/>
-    <col min="23" max="23" width="16.77734375" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="16.81640625" customWidth="1"/>
+    <col min="18" max="18" width="19.453125" customWidth="1"/>
+    <col min="19" max="19" width="17.08984375" customWidth="1"/>
+    <col min="20" max="20" width="19.453125" customWidth="1"/>
+    <col min="21" max="21" width="19.36328125" customWidth="1"/>
+    <col min="22" max="22" width="17.1796875" customWidth="1"/>
+    <col min="23" max="23" width="16.81640625" customWidth="1"/>
+    <col min="24" max="24" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>4</v>
@@ -1226,7 +1226,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
@@ -1240,13 +1240,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>38</v>
@@ -1294,7 +1294,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
aanpassing multi-link disruptie voor rws project en check voor bestaande pickle en graaf
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RA2CE_Sprint\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C59A46-5992-49FD-A078-1196EACA34BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC43E45E-EFF3-4374-8489-C2B5C96DC3D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
   <si>
     <t>analysis</t>
   </si>
@@ -164,9 +164,6 @@
     <t>by default, take all files in the folder ending *.tif, or *.shp</t>
   </si>
   <si>
-    <t>in case of .shp hazard map indicate the column</t>
-  </si>
-  <si>
     <t>in case of multiple analyses, separate by column</t>
   </si>
   <si>
@@ -267,13 +264,28 @@
   </si>
   <si>
     <t>TestNL</t>
+  </si>
+  <si>
+    <t>scenario_13794_wgs84.tif</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>in case of .shp hazard map indicate the column, in case of .tif come up with the variable name that you want it to becalled</t>
+  </si>
+  <si>
+    <t>Pavement_avg_depth</t>
+  </si>
+  <si>
+    <t>Multi-link Disruption_RWS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +325,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -349,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -384,6 +402,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,14 +737,14 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="21.54296875" customWidth="1"/>
     <col min="7" max="7" width="20.54296875" customWidth="1"/>
@@ -733,7 +754,7 @@
     <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
-    <col min="14" max="14" width="18.453125" customWidth="1"/>
+    <col min="14" max="14" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="22.1796875" customWidth="1"/>
     <col min="17" max="17" width="21.81640625" customWidth="1"/>
     <col min="18" max="18" width="20.6328125" customWidth="1"/>
@@ -745,7 +766,7 @@
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -762,7 +783,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -771,13 +792,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -786,55 +807,55 @@
         <v>8</v>
       </c>
       <c r="N1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="15" t="s">
-        <v>58</v>
-      </c>
       <c r="W1" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24">
       <c r="A2" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -845,21 +866,31 @@
         <v>25</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
+      <c r="Q2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0.1</v>
+      </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -885,7 +916,7 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -916,7 +947,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{09DA9868-2E07-4E38-A243-EA3D29C1341A}">
           <x14:formula1>
             <xm:f>options!$A$2:$A$4</xm:f>
@@ -927,7 +958,7 @@
           <x14:formula1>
             <xm:f>options!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>C3:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB96EDCB-7778-4C24-A755-D3846759BEB7}">
           <x14:formula1>
@@ -959,6 +990,12 @@
           </x14:formula1>
           <xm:sqref>R2:R1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1ECB901C-9956-47BD-8AF1-292DD6515458}">
+          <x14:formula1>
+            <xm:f>options!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -970,10 +1007,10 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.08984375" bestFit="1" customWidth="1"/>
@@ -982,7 +1019,7 @@
     <col min="7" max="7" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1002,10 +1039,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1022,13 +1059,13 @@
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -1045,13 +1082,13 @@
         <v>19</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -1068,26 +1105,28 @@
         <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="B5" s="18" t="s">
+        <v>80</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1096,18 +1135,18 @@
         <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -1121,11 +1160,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8FA5B4-8351-441E-BC93-E5502E84268F}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
@@ -1152,7 +1191,7 @@
     <col min="24" max="24" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="87">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1169,7 +1208,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>4</v>
@@ -1199,7 +1238,7 @@
         <v>33</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>34</v>
@@ -1211,22 +1250,22 @@
         <v>36</v>
       </c>
       <c r="T1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="V1" s="15" t="s">
-        <v>58</v>
-      </c>
       <c r="W1" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X1" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="116">
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
@@ -1240,13 +1279,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>38</v>
@@ -1266,37 +1305,37 @@
         <v>41</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="12" t="s">
-        <v>44</v>
-      </c>
       <c r="T2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="V2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="W2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
         <v>61</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ra2ce.py en analyses_indirect.py aangepast aan het RWS format. User input ook de optie voor RWS toegevoegd.
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RA2CE_Sprint\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC43E45E-EFF3-4374-8489-C2B5C96DC3D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973A3538-3C58-4788-BF1A-A9A61E677BF9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="92">
   <si>
     <t>analysis</t>
   </si>
@@ -263,9 +263,6 @@
     <t>NL_with_margin_from_EU_dump.osm.pbf</t>
   </si>
   <si>
-    <t>TestNL</t>
-  </si>
-  <si>
     <t>scenario_13794_wgs84.tif</t>
   </si>
   <si>
@@ -279,6 +276,42 @@
   </si>
   <si>
     <t>Multi-link Disruption_RWS</t>
+  </si>
+  <si>
+    <t>hazard_pickle</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_13794.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_13157.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_13165.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_13173.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_13812.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_13813.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_13814.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_13944.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_14013.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_19808.p</t>
+  </si>
+  <si>
+    <t>road_gdf_sel_20881.p</t>
   </si>
 </sst>
 </file>
@@ -734,39 +767,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.54296875" customWidth="1"/>
-    <col min="7" max="7" width="20.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="62.7265625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.08984375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="37.1796875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6328125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
     <col min="14" max="14" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="22.1796875" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="20.6328125" customWidth="1"/>
-    <col min="19" max="19" width="16.90625" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="17.90625" customWidth="1"/>
-    <col min="22" max="22" width="26.36328125" customWidth="1"/>
-    <col min="23" max="23" width="13.6328125" customWidth="1"/>
-    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="22.1796875" customWidth="1"/>
+    <col min="18" max="18" width="21.81640625" customWidth="1"/>
+    <col min="19" max="19" width="20.6328125" customWidth="1"/>
+    <col min="20" max="20" width="16.90625" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="22" max="22" width="17.90625" customWidth="1"/>
+    <col min="23" max="23" width="26.36328125" customWidth="1"/>
+    <col min="24" max="24" width="13.6328125" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -813,42 +847,45 @@
         <v>51</v>
       </c>
       <c r="P1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="17" t="s">
+      <c r="Y1" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="5" t="s">
-        <v>75</v>
+    <row r="2" spans="1:25">
+      <c r="A2" s="5">
+        <v>13157</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
@@ -869,78 +906,559 @@
         <v>49</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="5">
+      <c r="T2" s="5">
         <v>0.1</v>
       </c>
-      <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="Y2" s="5"/>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="5">
+        <v>13165</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="R3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0.1</v>
+      </c>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
-    </row>
-    <row r="4" spans="1:24">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="Y3" s="5"/>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="5">
+        <v>13173</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+      <c r="L4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="R4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0.1</v>
+      </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="5">
+        <v>13794</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="5">
+        <v>13812</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="5">
+        <v>13813</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="5">
+        <v>13814</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="5">
+        <v>13944</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="5">
+        <v>14013</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="5">
+        <v>19808</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T11" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="5">
+        <v>20881</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -958,7 +1476,7 @@
           <x14:formula1>
             <xm:f>options!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C1048576</xm:sqref>
+          <xm:sqref>C13:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB96EDCB-7778-4C24-A755-D3846759BEB7}">
           <x14:formula1>
@@ -988,13 +1506,13 @@
           <x14:formula1>
             <xm:f>options!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:R1048576</xm:sqref>
+          <xm:sqref>S2:S1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1ECB901C-9956-47BD-8AF1-292DD6515458}">
           <x14:formula1>
             <xm:f>options!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>C2:C12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1114,7 +1632,7 @@
     <row r="5" spans="1:7">
       <c r="A5" s="7"/>
       <c r="B5" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1305,7 +1823,7 @@
         <v>41</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
RWS project, de omreisroutes incl uitval van het onderliggende net.
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RA2CE_Sprint\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973A3538-3C58-4788-BF1A-A9A61E677BF9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9F397E-E63C-4A3C-9577-109514D4DC60}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="96">
   <si>
     <t>analysis</t>
   </si>
@@ -281,37 +281,49 @@
     <t>hazard_pickle</t>
   </si>
   <si>
-    <t>road_gdf_sel_13794.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_13157.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_13165.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_13173.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_13812.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_13813.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_13814.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_13944.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_14013.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_19808.p</t>
-  </si>
-  <si>
-    <t>road_gdf_sel_20881.p</t>
+    <t>including_underlying/road_gdf_sel_incl_underl13944.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13946.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl70012.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13814.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13813.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13943.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl70009.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13165.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl14013.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13173.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl19559.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13945.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13937.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13812.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl19558.p</t>
   </si>
 </sst>
 </file>
@@ -767,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -778,25 +790,27 @@
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7265625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="62.7265625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="27.08984375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="21.54296875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="37.1796875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="20.54296875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13.81640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6328125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="17.1796875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
     <col min="14" max="14" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="22.1796875" customWidth="1"/>
+    <col min="15" max="15" width="22.1796875" customWidth="1"/>
+    <col min="16" max="16" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.1796875" customWidth="1"/>
     <col min="18" max="18" width="21.81640625" customWidth="1"/>
-    <col min="19" max="19" width="20.6328125" customWidth="1"/>
-    <col min="20" max="20" width="16.90625" customWidth="1"/>
+    <col min="19" max="19" width="20.54296875" customWidth="1"/>
+    <col min="20" max="20" width="16.81640625" customWidth="1"/>
     <col min="21" max="21" width="12" customWidth="1"/>
-    <col min="22" max="22" width="17.90625" customWidth="1"/>
-    <col min="23" max="23" width="26.36328125" customWidth="1"/>
-    <col min="24" max="24" width="13.6328125" customWidth="1"/>
+    <col min="22" max="22" width="17.81640625" customWidth="1"/>
+    <col min="23" max="23" width="26.453125" customWidth="1"/>
+    <col min="24" max="24" width="13.54296875" customWidth="1"/>
     <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -879,7 +893,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="5">
-        <v>13157</v>
+        <v>13944</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -912,7 +926,7 @@
         <v>78</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="5" t="s">
@@ -932,7 +946,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="5">
-        <v>13165</v>
+        <v>13946</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>15</v>
@@ -965,7 +979,7 @@
         <v>78</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="5" t="s">
@@ -985,7 +999,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="5">
-        <v>13173</v>
+        <v>70012</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
@@ -1018,7 +1032,7 @@
         <v>78</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5" t="s">
@@ -1038,7 +1052,7 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="5">
-        <v>13794</v>
+        <v>13814</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>15</v>
@@ -1071,7 +1085,7 @@
         <v>78</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5" t="s">
@@ -1091,7 +1105,7 @@
     </row>
     <row r="6" spans="1:25">
       <c r="A6" s="5">
-        <v>13812</v>
+        <v>13813</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>15</v>
@@ -1144,7 +1158,7 @@
     </row>
     <row r="7" spans="1:25">
       <c r="A7" s="5">
-        <v>13813</v>
+        <v>13943</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -1197,7 +1211,7 @@
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="5">
-        <v>13814</v>
+        <v>70009</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
@@ -1250,7 +1264,7 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="5">
-        <v>13944</v>
+        <v>13165</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>15</v>
@@ -1356,7 +1370,7 @@
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="5">
-        <v>19808</v>
+        <v>13173</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>15</v>
@@ -1409,7 +1423,7 @@
     </row>
     <row r="12" spans="1:25">
       <c r="A12" s="5">
-        <v>20881</v>
+        <v>19559</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>15</v>
@@ -1459,6 +1473,218 @@
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="5">
+        <v>13945</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="5">
+        <v>13937</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T14" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="5">
+        <v>13812</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="5">
+        <v>19558</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T16" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1476,7 +1702,7 @@
           <x14:formula1>
             <xm:f>options!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C13:C1048576</xm:sqref>
+          <xm:sqref>C17:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB96EDCB-7778-4C24-A755-D3846759BEB7}">
           <x14:formula1>
@@ -1512,7 +1738,7 @@
           <x14:formula1>
             <xm:f>options!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C12</xm:sqref>
+          <xm:sqref>C2:C16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1531,8 +1757,8 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.81640625" customWidth="1"/>
   </cols>
@@ -1685,28 +1911,26 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.08984375" customWidth="1"/>
-    <col min="7" max="7" width="20.1796875" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.1796875" customWidth="1"/>
     <col min="8" max="8" width="22.54296875" customWidth="1"/>
-    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" customWidth="1"/>
     <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.1796875" customWidth="1"/>
-    <col min="14" max="14" width="22.6328125" customWidth="1"/>
+    <col min="14" max="14" width="22.54296875" customWidth="1"/>
     <col min="15" max="16" width="18" customWidth="1"/>
     <col min="17" max="17" width="16.81640625" customWidth="1"/>
     <col min="18" max="18" width="19.453125" customWidth="1"/>
-    <col min="19" max="19" width="17.08984375" customWidth="1"/>
-    <col min="20" max="20" width="19.453125" customWidth="1"/>
-    <col min="21" max="21" width="19.36328125" customWidth="1"/>
+    <col min="19" max="19" width="17.1796875" customWidth="1"/>
+    <col min="20" max="21" width="19.453125" customWidth="1"/>
     <col min="22" max="22" width="17.1796875" customWidth="1"/>
     <col min="23" max="23" width="16.81640625" customWidth="1"/>
-    <col min="24" max="24" width="16.36328125" customWidth="1"/>
+    <col min="24" max="24" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="87">

</xml_diff>

<commit_message>
Inclusief de koppeling aan verkeersintensiteiten voor het RWS project.
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RA2CE_Sprint\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9F397E-E63C-4A3C-9577-109514D4DC60}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C3792F-2381-437D-BC82-1914C8401D0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
   <si>
     <t>analysis</t>
   </si>
@@ -281,49 +281,7 @@
     <t>hazard_pickle</t>
   </si>
   <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13944.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13946.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl70012.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13814.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13813.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13943.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl70009.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13165.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl14013.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13173.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl19559.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13945.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl13937.p</t>
-  </si>
-  <si>
     <t>including_underlying/road_gdf_sel_incl_underl13812.p</t>
-  </si>
-  <si>
-    <t>including_underlying/road_gdf_sel_incl_underl19558.p</t>
   </si>
 </sst>
 </file>
@@ -779,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -893,7 +851,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="5">
-        <v>13944</v>
+        <v>13812</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -944,765 +902,29 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
     </row>
-    <row r="3" spans="1:25">
-      <c r="A3" s="5">
-        <v>13946</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="A4" s="5">
-        <v>70012</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="A5" s="5">
-        <v>13814</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T5" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="A6" s="5">
-        <v>13813</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T6" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" s="5">
-        <v>13943</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T7" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-    </row>
-    <row r="8" spans="1:25">
-      <c r="A8" s="5">
-        <v>70009</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T8" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-    </row>
-    <row r="9" spans="1:25">
-      <c r="A9" s="5">
-        <v>13165</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T9" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-    </row>
-    <row r="10" spans="1:25">
-      <c r="A10" s="5">
-        <v>14013</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T10" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-    </row>
-    <row r="11" spans="1:25">
-      <c r="A11" s="5">
-        <v>13173</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T11" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-    </row>
-    <row r="12" spans="1:25">
-      <c r="A12" s="5">
-        <v>19559</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T12" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-    </row>
-    <row r="13" spans="1:25">
-      <c r="A13" s="5">
-        <v>13945</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P13" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T13" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" s="5">
-        <v>13937</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P14" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T14" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="A15" s="5">
-        <v>13812</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P15" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T15" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-    </row>
-    <row r="16" spans="1:25">
-      <c r="A16" s="5">
-        <v>19558</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T16" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49CE237E-9A54-4C15-A1A1-5E22B2A25C3F}">
+          <x14:formula1>
+            <xm:f>options!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1ECB901C-9956-47BD-8AF1-292DD6515458}">
+          <x14:formula1>
+            <xm:f>options!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{09DA9868-2E07-4E38-A243-EA3D29C1341A}">
           <x14:formula1>
             <xm:f>options!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49CE237E-9A54-4C15-A1A1-5E22B2A25C3F}">
-          <x14:formula1>
-            <xm:f>options!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C17:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB96EDCB-7778-4C24-A755-D3846759BEB7}">
           <x14:formula1>
@@ -1733,12 +955,6 @@
             <xm:f>options!$G$2:$G$4</xm:f>
           </x14:formula1>
           <xm:sqref>S2:S1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1ECB901C-9956-47BD-8AF1-292DD6515458}">
-          <x14:formula1>
-            <xm:f>options!$B$2:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
foutmelding van de uiterste nodes als O/D eruit gehaald en de user_input_tests.xlsx ingevuld met het testbestand.
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RA2CE_Sprint\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C3792F-2381-437D-BC82-1914C8401D0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D3F4051-A7E1-4670-B775-93D9B5693BD3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="96">
   <si>
     <t>analysis</t>
   </si>
@@ -281,7 +281,49 @@
     <t>hazard_pickle</t>
   </si>
   <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13944.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13946.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl70012.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13814.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13813.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13943.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl70009.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13165.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl14013.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13173.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl19559.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13945.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl13937.p</t>
+  </si>
+  <si>
     <t>including_underlying/road_gdf_sel_incl_underl13812.p</t>
+  </si>
+  <si>
+    <t>including_underlying/road_gdf_sel_incl_underl19558.p</t>
   </si>
 </sst>
 </file>
@@ -737,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -851,7 +893,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="5">
-        <v>13812</v>
+        <v>13944</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -902,29 +944,765 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
     </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="5">
+        <v>13946</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="5">
+        <v>70012</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="5">
+        <v>13814</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="5">
+        <v>13813</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="5">
+        <v>13943</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="5">
+        <v>70009</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="5">
+        <v>13165</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="5">
+        <v>14013</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" s="5">
+        <v>13173</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T11" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" s="5">
+        <v>19559</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T12" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" s="5">
+        <v>13945</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" s="5">
+        <v>13937</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T14" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="A15" s="5">
+        <v>13812</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="5">
+        <v>19558</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T16" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49CE237E-9A54-4C15-A1A1-5E22B2A25C3F}">
-          <x14:formula1>
-            <xm:f>options!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3:C1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1ECB901C-9956-47BD-8AF1-292DD6515458}">
-          <x14:formula1>
-            <xm:f>options!$B$2:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{09DA9868-2E07-4E38-A243-EA3D29C1341A}">
           <x14:formula1>
             <xm:f>options!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49CE237E-9A54-4C15-A1A1-5E22B2A25C3F}">
+          <x14:formula1>
+            <xm:f>options!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C17:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB96EDCB-7778-4C24-A755-D3846759BEB7}">
           <x14:formula1>
@@ -955,6 +1733,12 @@
             <xm:f>options!$G$2:$G$4</xm:f>
           </x14:formula1>
           <xm:sqref>S2:S1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1ECB901C-9956-47BD-8AF1-292DD6515458}">
+          <x14:formula1>
+            <xm:f>options!$B$2:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
werkende single link disruption. OSMnx versie 0.9. De multi_link_od_matrix -> geeft een foutmelding en moet nog uitgezocht. Debugger mode loopt hij vast op geheugen foutmelding.
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RunningProjects\FEM_RA2CE\ra2ce\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2B11C6-D0FE-4F93-9B00-0D323858B52A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF4C322-F38E-464A-9ED2-3A7BC5C468B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -748,7 +748,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,7 +859,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>23</v>
@@ -877,7 +877,7 @@
         <v>25</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>81</v>
@@ -923,7 +923,7 @@
           <x14:formula1>
             <xm:f>options!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C1048576</xm:sqref>
+          <xm:sqref>C3:C1048576 C2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB96EDCB-7778-4C24-A755-D3846759BEB7}">
           <x14:formula1>
@@ -947,7 +947,7 @@
           <x14:formula1>
             <xm:f>[user_input.xlsx]options!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C2 R2</xm:sqref>
+          <xm:sqref>R2 B2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F37B468-FC80-4253-AF94-8064268B20AC}">
           <x14:formula1>

</xml_diff>

<commit_message>
De meest recente versie die lotte ook gebruikt voor haar social inclusiveness analyse.
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RunningProjects\FEM_RA2CE\ra2ce\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF4C322-F38E-464A-9ED2-3A7BC5C468B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15067917-C736-4581-AA7B-C6E06DBAE877}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
-    <sheet name="options" sheetId="2" r:id="rId2"/>
-    <sheet name="explanation" sheetId="3" r:id="rId3"/>
+    <sheet name="explanation" sheetId="3" r:id="rId2"/>
+    <sheet name="options" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
   <si>
     <t>analysis</t>
   </si>
@@ -177,18 +176,6 @@
     <t>snapping_threshold</t>
   </si>
   <si>
-    <t>motorway, trunk, primary, secondary, tertiary</t>
-  </si>
-  <si>
-    <t>motorway, trunk, primary, secondary</t>
-  </si>
-  <si>
-    <t>motorway, trunk, primary</t>
-  </si>
-  <si>
-    <t>motorway, trunk</t>
-  </si>
-  <si>
     <t>motorway</t>
   </si>
   <si>
@@ -231,9 +218,6 @@
     <t>segmentation</t>
   </si>
   <si>
-    <t>&lt;add another option here&gt;</t>
-  </si>
-  <si>
     <t>You can define the size of the segments the road will be cut into. When nothing is filled in, this step will be skipped</t>
   </si>
   <si>
@@ -264,9 +248,6 @@
     <t>name_of_pbf</t>
   </si>
   <si>
-    <t>case_extent_myanmar_manday</t>
-  </si>
-  <si>
     <t>waterdepth</t>
   </si>
   <si>
@@ -282,10 +263,40 @@
     <t>fid</t>
   </si>
   <si>
-    <t>merged_flood_week_31_mandalay.tif</t>
-  </si>
-  <si>
-    <t>test_myanmar</t>
+    <t>myanmar-latest.osm.pbf</t>
+  </si>
+  <si>
+    <t>motorway,trunk,primary,secondary,tertiary</t>
+  </si>
+  <si>
+    <t>motorway,trunk,primary,secondary</t>
+  </si>
+  <si>
+    <t>motorway,trunk,primary</t>
+  </si>
+  <si>
+    <t>motorway,trunk</t>
+  </si>
+  <si>
+    <t>merged_flood_week_29_mandalay.tif</t>
+  </si>
+  <si>
+    <t>motorway,motorway_link,trunk,trunk_link,primary,primary_link,secondary,secondary_link,tertiary,tertiary_link</t>
+  </si>
+  <si>
+    <t>motorway,motorway_link,trunk,trunk_link,primary,primary_link,secondary,secondary_link</t>
+  </si>
+  <si>
+    <t>motorway,motorway_link,trunk,trunk_link,primary,primary_link</t>
+  </si>
+  <si>
+    <t>motorway,motorway_link,trunk,trunk_link</t>
+  </si>
+  <si>
+    <t>motorway,motorway_link</t>
+  </si>
+  <si>
+    <t>test_mandalay</t>
   </si>
 </sst>
 </file>
@@ -341,7 +352,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -364,11 +375,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -403,6 +423,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,19 +443,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="options"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -748,32 +757,32 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="21.54296875" customWidth="1"/>
     <col min="7" max="7" width="20.54296875" customWidth="1"/>
     <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
     <col min="14" max="14" width="18.453125" customWidth="1"/>
     <col min="15" max="16" width="22.1796875" customWidth="1"/>
     <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="20.6328125" customWidth="1"/>
-    <col min="19" max="19" width="16.90625" customWidth="1"/>
+    <col min="18" max="18" width="20.54296875" customWidth="1"/>
+    <col min="19" max="19" width="16.81640625" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="17.90625" customWidth="1"/>
-    <col min="22" max="22" width="26.36328125" customWidth="1"/>
-    <col min="23" max="23" width="13.6328125" customWidth="1"/>
+    <col min="21" max="21" width="17.81640625" customWidth="1"/>
+    <col min="22" max="22" width="26.453125" customWidth="1"/>
+    <col min="23" max="23" width="13.54296875" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -794,7 +803,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -803,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -818,94 +827,86 @@
         <v>8</v>
       </c>
       <c r="N1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="T1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q1" s="14" t="s">
+      <c r="U1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="V1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="V1" s="15" t="s">
-        <v>58</v>
-      </c>
       <c r="W1" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>82</v>
+      <c r="A2" t="s">
+        <v>86</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
       <c r="L2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="M2" t="s">
         <v>81</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="R2" s="5" t="s">
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="5">
-        <v>0</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
+      <c r="S2">
+        <v>0.1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -919,47 +920,47 @@
           </x14:formula1>
           <xm:sqref>B3:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49CE237E-9A54-4C15-A1A1-5E22B2A25C3F}">
-          <x14:formula1>
-            <xm:f>options!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3:C1048576 C2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB96EDCB-7778-4C24-A755-D3846759BEB7}">
-          <x14:formula1>
-            <xm:f>options!$C$2:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6BB6EF60-BAF9-428D-B5C4-8EF858760B90}">
-          <x14:formula1>
-            <xm:f>options!$E$2:$E$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1D725D8C-87A9-4009-853D-1C43F6BFD1B9}">
           <x14:formula1>
             <xm:f>options!$G$2:$G$4</xm:f>
           </x14:formula1>
           <xm:sqref>R3:R1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{37956627-F8CC-4F06-8083-201D08419C46}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49CE237E-9A54-4C15-A1A1-5E22B2A25C3F}">
           <x14:formula1>
-            <xm:f>[user_input.xlsx]options!#REF!</xm:f>
+            <xm:f>options!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>R2 B2</xm:sqref>
+          <xm:sqref>C3:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB96EDCB-7778-4C24-A755-D3846759BEB7}">
+          <x14:formula1>
+            <xm:f>options!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6BB6EF60-BAF9-428D-B5C4-8EF858760B90}">
+          <x14:formula1>
+            <xm:f>options!$E$2:$E$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>L3:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F37B468-FC80-4253-AF94-8064268B20AC}">
           <x14:formula1>
             <xm:f>options!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>J3:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B14F2C85-AD67-4794-B3E8-7DE4537520AF}">
           <x14:formula1>
             <xm:f>options!$F$2:$F$7</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M1048576</xm:sqref>
+          <xm:sqref>M3:M1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B738E98-986C-4B32-87FD-8C705677A106}">
+          <x14:formula1>
+            <xm:f>options!$F$2:$F$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -968,190 +969,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB03C308-BA7F-4A52-B7FB-2322DB47837C}">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8FA5B4-8351-441E-BC93-E5502E84268F}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.08984375" customWidth="1"/>
-    <col min="7" max="7" width="20.1796875" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.1796875" customWidth="1"/>
     <col min="8" max="8" width="22.54296875" customWidth="1"/>
-    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" customWidth="1"/>
     <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.1796875" customWidth="1"/>
-    <col min="14" max="14" width="22.6328125" customWidth="1"/>
+    <col min="14" max="14" width="22.54296875" customWidth="1"/>
     <col min="15" max="16" width="18" customWidth="1"/>
     <col min="17" max="17" width="16.81640625" customWidth="1"/>
     <col min="18" max="18" width="19.453125" customWidth="1"/>
-    <col min="19" max="19" width="17.08984375" customWidth="1"/>
-    <col min="20" max="20" width="19.453125" customWidth="1"/>
-    <col min="21" max="21" width="19.36328125" customWidth="1"/>
+    <col min="19" max="19" width="17.1796875" customWidth="1"/>
+    <col min="20" max="21" width="19.453125" customWidth="1"/>
     <col min="22" max="22" width="17.1796875" customWidth="1"/>
     <col min="23" max="23" width="16.81640625" customWidth="1"/>
-    <col min="24" max="24" width="16.36328125" customWidth="1"/>
+    <col min="24" max="24" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="87" x14ac:dyDescent="0.35">
@@ -1171,7 +1018,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>4</v>
@@ -1201,7 +1048,7 @@
         <v>33</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>34</v>
@@ -1213,19 +1060,19 @@
         <v>36</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="X1" s="16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
@@ -1242,13 +1089,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>38</v>
@@ -1271,7 +1118,7 @@
         <v>42</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="12" t="s">
@@ -1281,24 +1128,24 @@
         <v>44</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="U2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="W2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="X2" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1317,4 +1164,176 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB03C308-BA7F-4A52-B7FB-2322DB47837C}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F9" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update first full day RA2CE sprint July 2021 - Single link redundancy from OSM download works!
</commit_message>
<xml_diff>
--- a/input/user_input_tests.xlsx
+++ b/input/user_input_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RunningProjects\FEM_RA2CE\ra2ce\ra2ce\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ceMaster\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15067917-C736-4581-AA7B-C6E06DBAE877}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33C7C22-DA3B-4E1C-92CD-7611F4C86DBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -756,37 +756,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.54296875" customWidth="1"/>
-    <col min="7" max="7" width="20.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="5" max="6" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
-    <col min="14" max="14" width="18.453125" customWidth="1"/>
-    <col min="15" max="16" width="22.1796875" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" customWidth="1"/>
-    <col min="18" max="18" width="20.54296875" customWidth="1"/>
-    <col min="19" max="19" width="16.81640625" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="16" width="22.21875" customWidth="1"/>
+    <col min="17" max="17" width="21.77734375" customWidth="1"/>
+    <col min="18" max="18" width="20.5546875" customWidth="1"/>
+    <col min="19" max="19" width="16.77734375" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="17.81640625" customWidth="1"/>
-    <col min="22" max="22" width="26.453125" customWidth="1"/>
-    <col min="23" max="23" width="13.54296875" customWidth="1"/>
+    <col min="21" max="21" width="17.77734375" customWidth="1"/>
+    <col min="22" max="22" width="26.44140625" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -860,7 +860,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -976,32 +976,32 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.1796875" customWidth="1"/>
-    <col min="8" max="8" width="22.54296875" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.21875" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.1796875" customWidth="1"/>
-    <col min="14" max="14" width="22.54296875" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" customWidth="1"/>
+    <col min="14" max="14" width="22.5546875" customWidth="1"/>
     <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="16.81640625" customWidth="1"/>
-    <col min="18" max="18" width="19.453125" customWidth="1"/>
-    <col min="19" max="19" width="17.1796875" customWidth="1"/>
-    <col min="20" max="21" width="19.453125" customWidth="1"/>
-    <col min="22" max="22" width="17.1796875" customWidth="1"/>
-    <col min="23" max="23" width="16.81640625" customWidth="1"/>
-    <col min="24" max="24" width="16.453125" customWidth="1"/>
+    <col min="17" max="17" width="16.77734375" customWidth="1"/>
+    <col min="18" max="18" width="19.44140625" customWidth="1"/>
+    <col min="19" max="19" width="17.21875" customWidth="1"/>
+    <col min="20" max="21" width="19.44140625" customWidth="1"/>
+    <col min="22" max="22" width="17.21875" customWidth="1"/>
+    <col min="23" max="23" width="16.77734375" customWidth="1"/>
+    <col min="24" max="24" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1170,20 +1170,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB03C308-BA7F-4A52-B7FB-2322DB47837C}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1312,22 +1312,22 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F8" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F9" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>85</v>
       </c>

</xml_diff>